<commit_message>
se creo el servicio que cargara las notas credito recibidas del archivo a la base de datos
</commit_message>
<xml_diff>
--- a/public/formatos/Formato_Notas_Credito.xlsx
+++ b/public/formatos/Formato_Notas_Credito.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grupozentria-my.sharepoint.com/personal/edwin_gonzalez_zentria_com_co/Documents/CAI-CARTERA/ESTADOS DE CARTERA 2025/SALUD TOTAL/11 NOVIEMBRE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programacion\Tablero-Bots\Backend\public\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB6AF607-5060-422D-ABEB-E93A0309CAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034685C6-8D9A-4A7B-94D7-19DBBE531120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6BF74BD9-EA5F-4416-90C9-B17CCFE4FD3F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BF74BD9-EA5F-4416-90C9-B17CCFE4FD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Contr. DIC2024" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,17 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>TIPO</t>
   </si>
@@ -69,9 +70,6 @@
   </si>
   <si>
     <t>Se genera NC de Cartera según conciliación administrativa de glosa Régimen Contributivo el 29/07/2025, periodo 01/01/2024 a 31/12/2024 (Conciliación Grupo Zentria) con aceptación por parte de Avidanti del 18%, con visto bueno de Presidencia y Dirección Financiera.</t>
-  </si>
-  <si>
-    <t>GL</t>
   </si>
 </sst>
 </file>
@@ -79,10 +77,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot; $&quot;#,##0.00\ ;&quot; $-&quot;#,##0.00\ ;&quot; $-&quot;#\ ;@\ "/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot; $&quot;#,##0.00\ ;&quot; $-&quot;#,##0.00\ ;&quot; $-&quot;#\ ;@\ "/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,9 +225,9 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -241,7 +239,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -275,7 +273,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -571,14 +569,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE05878-CE0D-4D56-80AD-24EAC54A3464}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:XFD3738"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" customWidth="1"/>
@@ -593,7 +591,7 @@
     <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +615,7 @@
       <c r="J1" s="4"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -643,7 +641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -666,158 +664,6 @@
         <v>800130907</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1176856</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4">
-        <v>94311</v>
-      </c>
-      <c r="F4" s="5">
-        <v>179703</v>
-      </c>
-      <c r="G4" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1158921</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="4">
-        <v>92938</v>
-      </c>
-      <c r="F5" s="5">
-        <v>15840</v>
-      </c>
-      <c r="G5" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1190323</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5">
-        <v>5000</v>
-      </c>
-      <c r="G6" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1190323</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="4">
-        <v>105708</v>
-      </c>
-      <c r="F7" s="5">
-        <v>5100</v>
-      </c>
-      <c r="G7" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1190629</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="4">
-        <v>130243</v>
-      </c>
-      <c r="F8" s="5">
-        <v>10107</v>
-      </c>
-      <c r="G8" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1227197</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="4">
-        <v>134547</v>
-      </c>
-      <c r="F9" s="5">
-        <v>3888</v>
-      </c>
-      <c r="G9" s="4">
-        <v>800130907</v>
-      </c>
-      <c r="H9" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>